<commit_message>
Add #REF! test for external references in named ranges.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/externalreferences.xlsx
+++ b/EPPlusTest/Workbooks/externalreferences.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpf\Documents\DELME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,8 +16,12 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="ExternalNamedRange">[2]Sheet1!$C$10</definedName>
+  </definedNames>
+  <calcPr calcId="171027" calcMode="manual" concurrentManualCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,6 +87,7 @@
       <sheetName val="Sheet1"/>
       <sheetName val="Sheet2"/>
       <sheetName val="Sheet3"/>
+      <sheetName val="ExternalWorkbook"/>
     </sheetNames>
     <definedNames>
       <definedName name="NL"/>
@@ -91,6 +96,20 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -393,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F9"/>
+  <dimension ref="F9:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,6 +426,12 @@
         <v>"NavSql","CRONUS USA, Inc.","18","1","01121212"</v>
       </c>
     </row>
+    <row r="15" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f>SUM(ExternalNamedRange, D4)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>